<commit_message>
Update CIERRE GASTOS ADMINISTRATIVOS DICIEMBRE 2025.xlsx
</commit_message>
<xml_diff>
--- a/CIERRE GASTOS ADMINISTRATIVOS DICIEMBRE 2025.xlsx
+++ b/CIERRE GASTOS ADMINISTRATIVOS DICIEMBRE 2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\PAGOS DICIEMBRE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\PAGOS DICIEMBRE\CIERRE-PAGOS-DICIEMBRE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D85C4C-2F6B-4AFC-8422-D0F7B1615291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828E0968-C76C-46AE-8872-70B359D12F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6D111AC9-F4B5-4EE1-9519-BE4E4E92E24D}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="83">
   <si>
     <t>ID_OBLIGACION</t>
   </si>
@@ -244,6 +244,51 @@
   </si>
   <si>
     <t>CARRANZA CHILMAZA JORGE LUIS</t>
+  </si>
+  <si>
+    <t>TRANSPORTES Y MANIOBRAS S.C.R.L.</t>
+  </si>
+  <si>
+    <t>BUSY BIZ SOLUTIONS S.A.C.</t>
+  </si>
+  <si>
+    <t>FAMIP INDUSTRIAL S.A.C.</t>
+  </si>
+  <si>
+    <t>DORAL SOLUCIONES PERU E.I.R.L.</t>
+  </si>
+  <si>
+    <t>HINOSTROZA GOMEZ JOSE</t>
+  </si>
+  <si>
+    <t>REPRESENTACIONES E &amp; N PALOMINO S.A.C.</t>
+  </si>
+  <si>
+    <t>BONILLA PEREZ JHON ARMANDO</t>
+  </si>
+  <si>
+    <t>MAMANI MOGROVEJO RONDOLFO</t>
+  </si>
+  <si>
+    <t>encargado de pago</t>
+  </si>
+  <si>
+    <t>SIN PAGO</t>
+  </si>
+  <si>
+    <t>TORREJON REYES ROSA MICAELA</t>
+  </si>
+  <si>
+    <t>NARVAEZ YSELA MIRIAM</t>
+  </si>
+  <si>
+    <t>202507|202508|202509</t>
+  </si>
+  <si>
+    <t>RABANAL MISARI ANA MARIA</t>
+  </si>
+  <si>
+    <t>estudiocontable_palomino@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -677,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620BD549-6BD9-4566-86B2-4950053DB95E}">
   <dimension ref="A1:Q136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="L136" sqref="L136"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.050000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1801,174 +1846,348 @@
       <c r="Q22" s="3"/>
     </row>
     <row r="23" spans="1:17" s="5" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="4"/>
+      <c r="A23" s="3">
+        <v>76474794</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="3">
+        <v>20505874529</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="3">
+        <v>20505874529</v>
+      </c>
+      <c r="I23" s="4">
+        <v>46003</v>
+      </c>
       <c r="J23" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67.79661016949153</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="8"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
+        <v>12.203389830508474</v>
+      </c>
+      <c r="L23" s="8">
+        <v>80</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N23" s="3">
+        <v>202510</v>
+      </c>
       <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
+      <c r="P23" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="Q23" s="3"/>
     </row>
     <row r="24" spans="1:17" s="5" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="4"/>
+      <c r="A24" s="3">
+        <v>76477124</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="3">
+        <v>20603914296</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" s="3">
+        <v>20603914296</v>
+      </c>
+      <c r="I24" s="4">
+        <v>46003</v>
+      </c>
       <c r="J24" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>174.05084745762713</v>
       </c>
       <c r="K24" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="8"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
+        <v>31.329152542372881</v>
+      </c>
+      <c r="L24" s="8">
+        <v>205.38</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N24" s="3">
+        <v>202510</v>
+      </c>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
     </row>
     <row r="25" spans="1:17" s="5" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="4"/>
+      <c r="A25" s="3">
+        <v>76479084</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="3">
+        <v>20612463591</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" s="3">
+        <v>20612463591</v>
+      </c>
+      <c r="I25" s="4">
+        <v>46002</v>
+      </c>
       <c r="J25" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>107.62711864406781</v>
       </c>
       <c r="K25" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="8"/>
-      <c r="M25" s="3"/>
+        <v>19.372881355932204</v>
+      </c>
+      <c r="L25" s="8">
+        <v>127</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
+      <c r="O25" s="3">
+        <v>202510</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="Q25" s="3"/>
     </row>
     <row r="26" spans="1:17" s="5" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="4"/>
+      <c r="A26" s="3">
+        <v>76475076</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="3">
+        <v>20521886871</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" s="3">
+        <v>20521886871</v>
+      </c>
+      <c r="I26" s="4">
+        <v>46003</v>
+      </c>
       <c r="J26" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>147.45762711864407</v>
       </c>
       <c r="K26" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L26" s="8"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
+        <v>26.542372881355931</v>
+      </c>
+      <c r="L26" s="8">
+        <v>174</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" s="3">
+        <v>202510</v>
+      </c>
       <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
+      <c r="P26" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="Q26" s="3"/>
     </row>
     <row r="27" spans="1:17" s="5" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="4"/>
+      <c r="A27" s="3">
+        <v>76474019</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="3">
+        <v>41977629</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="3">
+        <v>10419776292</v>
+      </c>
+      <c r="I27" s="4">
+        <v>46003</v>
+      </c>
       <c r="J27" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>86.440677966101703</v>
       </c>
       <c r="K27" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L27" s="8"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
+        <v>15.559322033898306</v>
+      </c>
+      <c r="L27" s="8">
+        <v>102</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N27" s="3">
+        <v>202510</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="Q27" s="3"/>
     </row>
     <row r="28" spans="1:17" s="5" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="4"/>
+      <c r="A28" s="3">
+        <v>76477631</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="3">
+        <v>20606210176</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" s="3">
+        <v>20606210176</v>
+      </c>
+      <c r="I28" s="4">
+        <v>46003</v>
+      </c>
       <c r="J28" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>56.016949152542374</v>
       </c>
       <c r="K28" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L28" s="8"/>
-      <c r="M28" s="3"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L28" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
+      <c r="O28" s="3">
+        <v>202510</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="Q28" s="3"/>
     </row>
     <row r="29" spans="1:17" s="5" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="4"/>
+      <c r="B29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="3">
+        <v>20519499780</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" s="3">
+        <v>20519499780</v>
+      </c>
+      <c r="I29" s="4">
+        <v>46003</v>
+      </c>
       <c r="J29" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>455.64406779661016</v>
       </c>
       <c r="K29" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L29" s="8"/>
+        <v>82.015932203389823</v>
+      </c>
+      <c r="L29" s="8">
+        <v>537.66</v>
+      </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
@@ -1976,52 +2195,104 @@
       <c r="Q29" s="3"/>
     </row>
     <row r="30" spans="1:17" s="5" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="4"/>
+      <c r="A30" s="3">
+        <v>76473991</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="3">
+        <v>40721603</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H30" s="3">
+        <v>10407216038</v>
+      </c>
+      <c r="I30" s="4">
+        <v>46004</v>
+      </c>
       <c r="J30" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>78.084745762711876</v>
       </c>
       <c r="K30" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L30" s="8"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
+        <v>14.055254237288137</v>
+      </c>
+      <c r="L30" s="8">
+        <v>92.14</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N30" s="3">
+        <v>202510</v>
+      </c>
       <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
+      <c r="P30" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="Q30" s="3"/>
     </row>
     <row r="31" spans="1:17" s="5" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="4"/>
+      <c r="A31" s="3">
+        <v>76474057</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="3">
+        <v>43371623</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H31" s="3">
+        <v>10433716235</v>
+      </c>
+      <c r="I31" s="4">
+        <v>46004</v>
+      </c>
       <c r="J31" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>56.016949152542374</v>
       </c>
       <c r="K31" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L31" s="8"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L31" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N31" s="3">
+        <v>202510</v>
+      </c>
+      <c r="O31" s="3">
+        <v>202509</v>
+      </c>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
     </row>
@@ -4628,15 +4899,15 @@
     <row r="136" spans="1:17" s="5" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J136" s="11">
         <f>SUBTOTAL(9,J2:J135)</f>
-        <v>1831.5084745762711</v>
+        <v>3060.6440677966107</v>
       </c>
       <c r="K136" s="11">
         <f>SUBTOTAL(9,K2:K135)</f>
-        <v>329.67152542372878</v>
+        <v>550.91593220338973</v>
       </c>
       <c r="L136" s="11">
         <f>SUM(L2:L135)</f>
-        <v>2161.1799999999998</v>
+        <v>3611.5599999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>